<commit_message>
refix ZSS-901: find filter range.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/901-filter-range.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/901-filter-range.xlsx
@@ -16,6 +16,14 @@
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>a</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -345,15 +353,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:6">
       <c r="B2">
         <v>1</v>
       </c>
@@ -364,7 +372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:6">
       <c r="B3">
         <v>2</v>
       </c>
@@ -375,7 +383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:6">
       <c r="B4">
         <v>3</v>
       </c>
@@ -383,9 +391,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:6">
       <c r="C5">
         <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>